<commit_message>
Updated Generate PLC Code
</commit_message>
<xml_diff>
--- a/export/siemens/PLC_Textlist/MTR_Plc_alarm_Textlists.xlsx
+++ b/export/siemens/PLC_Textlist/MTR_Plc_alarm_Textlists.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="TextList" sheetId="1" r:id="rId1"/>
+    <sheet name="TextListEntry" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +33,54 @@
   </si>
   <si>
     <t>Item name for ControlModules</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Text [en-US]</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>Agitator Start</t>
+  </si>
+  <si>
+    <t>Circulation pump</t>
+  </si>
+  <si>
+    <t>Antifoam Pump</t>
+  </si>
+  <si>
+    <t>Base Pump</t>
+  </si>
+  <si>
+    <t>Feed Pump</t>
+  </si>
+  <si>
+    <t>Innoculum Pump</t>
   </si>
 </sst>
 </file>
@@ -420,4 +469,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for cloud version and add hmiand scada code
</commit_message>
<xml_diff>
--- a/export/siemens/PLC_Textlist/MTR_Plc_alarm_Textlists.xlsx
+++ b/export/siemens/PLC_Textlist/MTR_Plc_alarm_Textlists.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="TextList" sheetId="1" r:id="rId1"/>
+    <sheet name="TextListEntry" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +33,54 @@
   </si>
   <si>
     <t>Item name for ControlModules</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Text [en-US]</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>Agitator Start</t>
+  </si>
+  <si>
+    <t>Circulation pump</t>
+  </si>
+  <si>
+    <t>Antifoam Pump</t>
+  </si>
+  <si>
+    <t>Base Pump</t>
+  </si>
+  <si>
+    <t>Feed Pump</t>
+  </si>
+  <si>
+    <t>Innoculum Pump</t>
   </si>
 </sst>
 </file>
@@ -420,4 +469,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>